<commit_message>
Common: Extended some data
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/boosters.xlsx
+++ b/upgrade/fixtures/boosters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFAB4F3-4363-4E26-ACAF-58FEEE277E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C743B5-BD56-4B5C-A538-A9CBCE6B9DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="5490" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2010" yWindow="7965" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>tab</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>Nico Base Fifty</t>
+  </si>
+  <si>
+    <t>pg</t>
+  </si>
+  <si>
+    <t>vg</t>
   </si>
 </sst>
 </file>
@@ -435,10 +441,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BECEFDC-C527-407A-9BBF-AF98CD28B0D3}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,9 +453,11 @@
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -457,13 +465,19 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -471,13 +485,19 @@
         <v>9</v>
       </c>
       <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>70</v>
+      </c>
+      <c r="E2">
         <v>20</v>
       </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -485,13 +505,19 @@
         <v>9</v>
       </c>
       <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>70</v>
+      </c>
+      <c r="E3">
         <v>18</v>
       </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -499,13 +525,19 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -513,13 +545,19 @@
         <v>10</v>
       </c>
       <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+      <c r="E5">
         <v>20</v>
       </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -527,13 +565,19 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -541,13 +585,19 @@
         <v>10</v>
       </c>
       <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
+      <c r="E7">
         <v>12</v>
       </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -555,9 +605,15 @@
         <v>11</v>
       </c>
       <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
         <v>3</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>10</v>
       </c>
     </row>

</xml_diff>